<commit_message>
Integrate cell extractor with main module and first successful test
</commit_message>
<xml_diff>
--- a/Code/Final Code/Yarab.xlsx
+++ b/Code/Final Code/Yarab.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Code</t>
   </si>
@@ -34,16 +34,175 @@
     <t>3</t>
   </si>
   <si>
+    <t>1180236</t>
+  </si>
+  <si>
+    <t>احمد معتز لطفى احمد</t>
+  </si>
+  <si>
+    <t>Ahmed Motaaz Lotfy Ahmed</t>
+  </si>
+  <si>
+    <t>1180333</t>
+  </si>
+  <si>
+    <t>حبيبة عصام حسب الله توفيق عمران</t>
+  </si>
+  <si>
+    <t>Habiba Essam Hassaballah Tawfik Omran</t>
+  </si>
+  <si>
+    <t>1180128</t>
+  </si>
+  <si>
+    <t>سعد الذدين محمد سعد محمد</t>
+  </si>
+  <si>
+    <t>Saad El-din Mohamed Saad Mohamed</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>1180255</t>
   </si>
   <si>
+    <t>عبد الله محمد جلال السحيى</t>
+  </si>
+  <si>
+    <t>AbdAllah Mohammed Galal El-Suhaimi</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1180274</t>
+  </si>
+  <si>
+    <t>علا ايمن عبدالفتاح المغربى</t>
+  </si>
+  <si>
+    <t>Ola ayman abdelftah elmaghraby</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1180056</t>
+  </si>
+  <si>
+    <t>على شريف على حسب الله</t>
+  </si>
+  <si>
+    <t>Ali Sharif Ali Hasb Allah</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1180041</t>
+  </si>
+  <si>
+    <t>عمر محمد فتحى شلقاى شعراوى</t>
+  </si>
+  <si>
+    <t>Omar Mohamed Fathy Shalkkamy Shaarawy</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1180606</t>
+  </si>
+  <si>
     <t>فاطمة عصام محمد جاب الله</t>
   </si>
   <si>
+    <t>Fatma Issam Mohamed Gaballah</t>
+  </si>
+  <si>
+    <t>1180456</t>
+  </si>
+  <si>
+    <t>فرح اسامه زين الدين محمد</t>
+  </si>
+  <si>
+    <t>farah ossama zein elden</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2200022</t>
+  </si>
+  <si>
+    <t>محمد السيد احمد عبداللطيف</t>
+  </si>
+  <si>
     <t>Mohamed Elsayed Ahmed Abdellatif</t>
   </si>
   <si>
-    <t>9</t>
+    <t>1180552</t>
+  </si>
+  <si>
+    <t>محمد خالد محمد ابراهيم شمس</t>
+  </si>
+  <si>
+    <t>Mohamed Khaled Mohamed Ebrahim</t>
+  </si>
+  <si>
+    <t>1180207</t>
+  </si>
+  <si>
+    <t>محمد عبداللطيف محمد المصرى</t>
+  </si>
+  <si>
+    <t>Mohammed Abdul Latif Mohamed Ei Masry</t>
+  </si>
+  <si>
+    <t>1180045</t>
+  </si>
+  <si>
+    <t>مصطتى نضال مصطفى عزت حافظ</t>
+  </si>
+  <si>
+    <t>Mostafa Neddal Mostafa Ezzat Hafez</t>
+  </si>
+  <si>
+    <t>1180212</t>
+  </si>
+  <si>
+    <t>متار سمي ر كامل ابوهواش</t>
+  </si>
+  <si>
+    <t>Manar Samir Kamel AboHawash</t>
+  </si>
+  <si>
+    <t>1180155</t>
+  </si>
+  <si>
+    <t>ابو ال</t>
+  </si>
+  <si>
+    <t>Mennatallah Hisham Hassan Ahmed</t>
+  </si>
+  <si>
+    <t>1170343</t>
+  </si>
+  <si>
+    <t>وليد علاء فتحى انيس</t>
+  </si>
+  <si>
+    <t>Waleed Alaa Fathy Anees</t>
+  </si>
+  <si>
+    <t>1180172</t>
+  </si>
+  <si>
+    <t>ياسمين عمرو فاروق محمد رشاد</t>
+  </si>
+  <si>
+    <t>Yasmin Amr Farouk Mohamed Rashad</t>
   </si>
 </sst>
 </file>
@@ -59,18 +218,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -96,7 +249,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -433,11 +585,333 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>